<commit_message>
EPBDS-9859 More test cases
--HG--
branch : 5.23.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9859_invalid_chars _in_field_names.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9859_invalid_chars _in_field_names.xlsx
@@ -5,30 +5,35 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ybiruk\Desktop\new\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A69DFF0-503B-4AA6-B9BC-2709EA52D618}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E7F59C-4A4E-4316-8AE3-F6CF4FBBB2C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
-  <si>
-    <t>Datatype MyType</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t>String</t>
   </si>
@@ -36,9 +41,6 @@
     <t>array[]</t>
   </si>
   <si>
-    <t>String[]</t>
-  </si>
-  <si>
     <t>Datatype MyType2</t>
   </si>
   <si>
@@ -61,6 +63,66 @@
   </si>
   <si>
     <t>array*</t>
+  </si>
+  <si>
+    <t>массив</t>
+  </si>
+  <si>
+    <t>Datatype Массив</t>
+  </si>
+  <si>
+    <t>Массив</t>
+  </si>
+  <si>
+    <t>array²</t>
+  </si>
+  <si>
+    <t>0array</t>
+  </si>
+  <si>
+    <t>Datatype MyType1</t>
+  </si>
+  <si>
+    <t>Datatype Массив_2</t>
+  </si>
+  <si>
+    <t>Datatype MyType1_2</t>
+  </si>
+  <si>
+    <t>Datatype MyType2_2</t>
+  </si>
+  <si>
+    <t>Datatype MyType3_2</t>
+  </si>
+  <si>
+    <t>Datatype MyType4_2</t>
+  </si>
+  <si>
+    <t>Datatype MyType5_2</t>
+  </si>
+  <si>
+    <t>массив2</t>
+  </si>
+  <si>
+    <t>Datatype Массив_3</t>
+  </si>
+  <si>
+    <t>Datatype MyType1_3</t>
+  </si>
+  <si>
+    <t>Datatype MyType2_3</t>
+  </si>
+  <si>
+    <t>Datatype MyType3_3</t>
+  </si>
+  <si>
+    <t>Datatype MyType4_3</t>
+  </si>
+  <si>
+    <t>Datatype MyType5_3</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -100,7 +162,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -378,77 +440,276 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FC716B1-71C9-4388-A30F-D62CB75B97CB}">
-  <dimension ref="B3:C16"/>
+  <dimension ref="B3:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" t="str">
+        <f>C4 &amp;" :context"</f>
+        <v>_array :context</v>
+      </c>
+      <c r="J4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" ref="K4:K7" si="0">C4 &amp;" :context .lob"</f>
+        <v>_array :context .lob</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" ref="G5:G7" si="1">C5 &amp;" :context"</f>
+        <v>$array :context</v>
+      </c>
+      <c r="J5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" t="str">
+        <f>C5 &amp;" :context.nature"</f>
+        <v>$array :context.nature</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="str">
+        <f>C6 &amp;":context"</f>
+        <v>массив:context</v>
+      </c>
+      <c r="J6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" t="str">
+        <f>C6 &amp;":context.requestDate"</f>
+        <v>массив:context.requestDate</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="1"/>
+        <v>массив2 :context</v>
+      </c>
+      <c r="J7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" t="str">
+        <f>C7 &amp;" :context .lang"</f>
+        <v>массив2 :context .lang</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" ref="G10" si="2">C10 &amp;" :context"</f>
+        <v>array² :context</v>
+      </c>
+      <c r="J10" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" t="str">
+        <f>C10 &amp;" :context .lob"</f>
+        <v>array² :context .lob</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" ref="G13" si="3">C13 &amp;" :context"</f>
+        <v>0array :context</v>
+      </c>
+      <c r="J13" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13" t="str">
+        <f>C13 &amp;" :context .lob"</f>
+        <v>0array :context .lob</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="F16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" ref="G16" si="4">C16 &amp;" :context"</f>
+        <v>array[] :context</v>
+      </c>
+      <c r="J16" t="s">
+        <v>0</v>
+      </c>
+      <c r="K16" t="str">
+        <f>C16 &amp;" :context .lob"</f>
+        <v>array[] :context .lob</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="F19" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" ref="G19" si="5">C19 &amp;" :context"</f>
+        <v>array^ :context</v>
+      </c>
+      <c r="J19" t="s">
+        <v>0</v>
+      </c>
+      <c r="K19" t="str">
+        <f>C19 &amp;" :context .lob"</f>
+        <v>array^ :context .lob</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+      <c r="J21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" t="s">
-        <v>11</v>
+      <c r="F22" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" ref="G22" si="6">C22 &amp;" :context"</f>
+        <v>array* :context</v>
+      </c>
+      <c r="J22" t="s">
+        <v>0</v>
+      </c>
+      <c r="K22" t="str">
+        <f>C22 &amp;" :context .lob"</f>
+        <v>array* :context .lob</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EPBDS-9859 Not informative error message or not message at all is presented to user if datatype field name contains invalid chars
--HG--
branch : 5.23.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9859_invalid_chars _in_field_names.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9859_invalid_chars _in_field_names.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\openL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E7F59C-4A4E-4316-8AE3-F6CF4FBBB2C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E98AC7-2B70-4322-B725-AEA4EE285397}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист2" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>String</t>
   </si>
@@ -44,12 +44,6 @@
     <t>Datatype MyType2</t>
   </si>
   <si>
-    <t>_array</t>
-  </si>
-  <si>
-    <t>$array</t>
-  </si>
-  <si>
     <t>Datatype MyType3</t>
   </si>
   <si>
@@ -65,15 +59,6 @@
     <t>array*</t>
   </si>
   <si>
-    <t>массив</t>
-  </si>
-  <si>
-    <t>Datatype Массив</t>
-  </si>
-  <si>
-    <t>Массив</t>
-  </si>
-  <si>
     <t>array²</t>
   </si>
   <si>
@@ -83,9 +68,6 @@
     <t>Datatype MyType1</t>
   </si>
   <si>
-    <t>Datatype Массив_2</t>
-  </si>
-  <si>
     <t>Datatype MyType1_2</t>
   </si>
   <si>
@@ -101,12 +83,6 @@
     <t>Datatype MyType5_2</t>
   </si>
   <si>
-    <t>массив2</t>
-  </si>
-  <si>
-    <t>Datatype Массив_3</t>
-  </si>
-  <si>
     <t>Datatype MyType1_3</t>
   </si>
   <si>
@@ -120,9 +96,6 @@
   </si>
   <si>
     <t>Datatype MyType5_3</t>
-  </si>
-  <si>
-    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -162,7 +135,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -440,23 +413,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FC716B1-71C9-4388-A30F-D62CB75B97CB}">
-  <dimension ref="B3:K22"/>
+  <dimension ref="B3:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
+      <c r="J3" t="s">
         <v>16</v>
-      </c>
-      <c r="J3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
@@ -464,98 +437,65 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
         <v>0</v>
       </c>
       <c r="G4" t="str">
-        <f>C4 &amp;" :context"</f>
-        <v>_array :context</v>
+        <f t="shared" ref="G4" si="0">C4 &amp;" :context"</f>
+        <v>array² :context</v>
       </c>
       <c r="J4" t="s">
         <v>0</v>
       </c>
       <c r="K4" t="str">
-        <f t="shared" ref="K4:K7" si="0">C4 &amp;" :context .lob"</f>
-        <v>_array :context .lob</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" t="str">
-        <f t="shared" ref="G5:G7" si="1">C5 &amp;" :context"</f>
-        <v>$array :context</v>
-      </c>
-      <c r="J5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K5" t="str">
-        <f>C5 &amp;" :context.nature"</f>
-        <v>$array :context.nature</v>
+        <f>C4 &amp;" :context .lob"</f>
+        <v>array² :context .lob</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" t="str">
-        <f>C6 &amp;":context"</f>
-        <v>массив:context</v>
+        <v>12</v>
       </c>
       <c r="J6" t="s">
-        <v>29</v>
-      </c>
-      <c r="K6" t="str">
-        <f>C6 &amp;":context.requestDate"</f>
-        <v>массив:context.requestDate</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G7" t="str">
-        <f t="shared" si="1"/>
-        <v>массив2 :context</v>
+        <f t="shared" ref="G7" si="1">C7 &amp;" :context"</f>
+        <v>0array :context</v>
       </c>
       <c r="J7" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K7" t="str">
-        <f>C7 &amp;" :context .lang"</f>
-        <v>массив2 :context .lang</v>
+        <f>C7 &amp;" :context .lob"</f>
+        <v>0array :context .lob</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J9" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
@@ -563,32 +503,32 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="F10" t="s">
         <v>0</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" ref="G10" si="2">C10 &amp;" :context"</f>
-        <v>array² :context</v>
+        <v>array[] :context</v>
       </c>
       <c r="J10" t="s">
         <v>0</v>
       </c>
       <c r="K10" t="str">
         <f>C10 &amp;" :context .lob"</f>
-        <v>array² :context .lob</v>
+        <v>array[] :context .lob</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J12" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
@@ -596,32 +536,32 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F13" t="s">
         <v>0</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" ref="G13" si="3">C13 &amp;" :context"</f>
-        <v>0array :context</v>
+        <v>array^ :context</v>
       </c>
       <c r="J13" t="s">
         <v>0</v>
       </c>
       <c r="K13" t="str">
         <f>C13 &amp;" :context .lob"</f>
-        <v>0array :context .lob</v>
+        <v>array^ :context .lob</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F15" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="J15" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
@@ -629,86 +569,20 @@
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F16" t="s">
         <v>0</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" ref="G16" si="4">C16 &amp;" :context"</f>
-        <v>array[] :context</v>
+        <v>array* :context</v>
       </c>
       <c r="J16" t="s">
         <v>0</v>
       </c>
       <c r="K16" t="str">
         <f>C16 &amp;" :context .lob"</f>
-        <v>array[] :context .lob</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" t="s">
-        <v>20</v>
-      </c>
-      <c r="J18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="F19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G19" t="str">
-        <f t="shared" ref="G19" si="5">C19 &amp;" :context"</f>
-        <v>array^ :context</v>
-      </c>
-      <c r="J19" t="s">
-        <v>0</v>
-      </c>
-      <c r="K19" t="str">
-        <f>C19 &amp;" :context .lob"</f>
-        <v>array^ :context .lob</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" t="s">
-        <v>21</v>
-      </c>
-      <c r="J21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" t="s">
-        <v>0</v>
-      </c>
-      <c r="G22" t="str">
-        <f t="shared" ref="G22" si="6">C22 &amp;" :context"</f>
-        <v>array* :context</v>
-      </c>
-      <c r="J22" t="s">
-        <v>0</v>
-      </c>
-      <c r="K22" t="str">
-        <f>C22 &amp;" :context .lob"</f>
         <v>array* :context .lob</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EPBDS-9859 Validate context property names as well
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9859_invalid_chars _in_field_names.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9859_invalid_chars _in_field_names.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\openL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E98AC7-2B70-4322-B725-AEA4EE285397}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D648A47-8F5A-4AAC-B7FE-8ADC0FFB3365}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист2" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
   <si>
     <t>String</t>
   </si>
@@ -44,6 +44,12 @@
     <t>Datatype MyType2</t>
   </si>
   <si>
+    <t>_array</t>
+  </si>
+  <si>
+    <t>$array</t>
+  </si>
+  <si>
     <t>Datatype MyType3</t>
   </si>
   <si>
@@ -59,6 +65,15 @@
     <t>array*</t>
   </si>
   <si>
+    <t>массив</t>
+  </si>
+  <si>
+    <t>Datatype Массив</t>
+  </si>
+  <si>
+    <t>Массив</t>
+  </si>
+  <si>
     <t>array²</t>
   </si>
   <si>
@@ -68,6 +83,9 @@
     <t>Datatype MyType1</t>
   </si>
   <si>
+    <t>Datatype Массив_2</t>
+  </si>
+  <si>
     <t>Datatype MyType1_2</t>
   </si>
   <si>
@@ -83,6 +101,12 @@
     <t>Datatype MyType5_2</t>
   </si>
   <si>
+    <t>массив2</t>
+  </si>
+  <si>
+    <t>Datatype Массив_3</t>
+  </si>
+  <si>
     <t>Datatype MyType1_3</t>
   </si>
   <si>
@@ -96,6 +120,12 @@
   </si>
   <si>
     <t>Datatype MyType5_3</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Datatype Массив_4</t>
   </si>
 </sst>
 </file>
@@ -135,7 +165,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -413,176 +443,306 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FC716B1-71C9-4388-A30F-D62CB75B97CB}">
-  <dimension ref="B3:K16"/>
+  <dimension ref="B3:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" t="str">
+        <f>C4 &amp;" :context"</f>
+        <v>_array :context</v>
+      </c>
+      <c r="J4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" ref="K4" si="0">C4 &amp;" :context .lob"</f>
+        <v>_array :context .lob</v>
+      </c>
+      <c r="N4" t="s">
+        <v>0</v>
+      </c>
+      <c r="O4" t="str">
+        <f>C4 &amp;" :context .0type"</f>
+        <v>_array :context .0type</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" ref="G5:G7" si="1">C5 &amp;" :context"</f>
+        <v>$array :context</v>
+      </c>
+      <c r="J5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" t="str">
+        <f>C5 &amp;" :context.nature"</f>
+        <v>$array :context.nature</v>
+      </c>
+      <c r="N5" t="s">
+        <v>0</v>
+      </c>
+      <c r="O5" t="str">
+        <f>C5 &amp;" :context .type*"</f>
+        <v>$array :context .type*</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" t="str">
-        <f t="shared" ref="G4" si="0">C4 &amp;" :context"</f>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="str">
+        <f>C6 &amp;":context"</f>
+        <v>массив:context</v>
+      </c>
+      <c r="J6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" t="str">
+        <f>C6 &amp;":context.requestDate"</f>
+        <v>массив:context.requestDate</v>
+      </c>
+      <c r="N6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O6" t="str">
+        <f>C6 &amp;" :context ."</f>
+        <v>массив :context .</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="1"/>
+        <v>массив2 :context</v>
+      </c>
+      <c r="J7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" t="str">
+        <f>C7 &amp;" :context .lang"</f>
+        <v>массив2 :context .lang</v>
+      </c>
+      <c r="N7" t="s">
+        <v>12</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" ref="O5:O7" si="2">C7 &amp;" :context .lob"</f>
+        <v>массив2 :context .lob</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" ref="G10" si="3">C10 &amp;" :context"</f>
         <v>array² :context</v>
-      </c>
-      <c r="J4" t="s">
-        <v>0</v>
-      </c>
-      <c r="K4" t="str">
-        <f>C4 &amp;" :context .lob"</f>
-        <v>array² :context .lob</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" t="str">
-        <f t="shared" ref="G7" si="1">C7 &amp;" :context"</f>
-        <v>0array :context</v>
-      </c>
-      <c r="J7" t="s">
-        <v>0</v>
-      </c>
-      <c r="K7" t="str">
-        <f>C7 &amp;" :context .lob"</f>
-        <v>0array :context .lob</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10" t="s">
-        <v>0</v>
-      </c>
-      <c r="G10" t="str">
-        <f t="shared" ref="G10" si="2">C10 &amp;" :context"</f>
-        <v>array[] :context</v>
       </c>
       <c r="J10" t="s">
         <v>0</v>
       </c>
       <c r="K10" t="str">
         <f>C10 &amp;" :context .lob"</f>
-        <v>array[] :context .lob</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+        <v>array² :context .lob</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
         <v>14</v>
       </c>
-      <c r="J12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
       <c r="F13" t="s">
         <v>0</v>
       </c>
       <c r="G13" t="str">
-        <f t="shared" ref="G13" si="3">C13 &amp;" :context"</f>
-        <v>array^ :context</v>
+        <f t="shared" ref="G13" si="4">C13 &amp;" :context"</f>
+        <v>0array :context</v>
       </c>
       <c r="J13" t="s">
         <v>0</v>
       </c>
       <c r="K13" t="str">
         <f>C13 &amp;" :context .lob"</f>
-        <v>array^ :context .lob</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+        <v>0array :context .lob</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F15" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F16" t="s">
         <v>0</v>
       </c>
       <c r="G16" t="str">
-        <f t="shared" ref="G16" si="4">C16 &amp;" :context"</f>
-        <v>array* :context</v>
+        <f t="shared" ref="G16" si="5">C16 &amp;" :context"</f>
+        <v>array[] :context</v>
       </c>
       <c r="J16" t="s">
         <v>0</v>
       </c>
       <c r="K16" t="str">
         <f>C16 &amp;" :context .lob"</f>
+        <v>array[] :context .lob</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" ref="G19" si="6">C19 &amp;" :context"</f>
+        <v>array^ :context</v>
+      </c>
+      <c r="J19" t="s">
+        <v>0</v>
+      </c>
+      <c r="K19" t="str">
+        <f>C19 &amp;" :context .lob"</f>
+        <v>array^ :context .lob</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+      <c r="J21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" ref="G22" si="7">C22 &amp;" :context"</f>
+        <v>array* :context</v>
+      </c>
+      <c r="J22" t="s">
+        <v>0</v>
+      </c>
+      <c r="K22" t="str">
+        <f>C22 &amp;" :context .lob"</f>
         <v>array* :context .lob</v>
       </c>
     </row>

</xml_diff>